<commit_message>
Alterado médias e gráfico por LIcitação, Dispensa e Registro de Preços
</commit_message>
<xml_diff>
--- a/SICOP 1.xlsx
+++ b/SICOP 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="11760" windowHeight="5280"/>
   </bookViews>
   <sheets>
     <sheet name="Plan2" sheetId="2" r:id="rId1"/>
     <sheet name="Plan3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -231,9 +231,6 @@
     <t>SECRETARIA DE FINANÇAS</t>
   </si>
   <si>
-    <t>ENCAMINHAR PARANDISPONIBILIDADE FINANCEIRA</t>
-  </si>
-  <si>
     <t>AUTORIZAÇÃO</t>
   </si>
   <si>
@@ -247,13 +244,16 @@
   </si>
   <si>
     <t>COORDENADORIA DE LICITAÇÃO</t>
+  </si>
+  <si>
+    <t>ENCAMINHAR PARA DISPONIBILIDADE FINANCEIRA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1297,6 +1297,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1331,6 +1332,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1506,14 +1508,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="4" width="11.42578125" customWidth="1"/>
@@ -1528,7 +1530,7 @@
     <col min="17" max="17" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
@@ -1549,7 +1551,7 @@
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1">
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -1568,7 +1570,7 @@
       <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
     </row>
-    <row r="4" spans="1:17" ht="16.5" thickTop="1">
+    <row r="4" spans="1:17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="25" t="s">
@@ -1597,7 +1599,7 @@
       <c r="P4" s="26"/>
       <c r="Q4" s="17"/>
     </row>
-    <row r="5" spans="1:17" ht="21.75" thickBot="1">
+    <row r="5" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="20" t="s">
@@ -1626,7 +1628,7 @@
       <c r="P5" s="21"/>
       <c r="Q5" s="19"/>
     </row>
-    <row r="6" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1">
+    <row r="6" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1645,7 +1647,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="7" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="29" t="s">
@@ -1674,7 +1676,7 @@
       <c r="P7" s="30"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1">
+    <row r="8" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
@@ -1693,7 +1695,7 @@
       <c r="P8" s="3"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="9" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="29" t="s">
@@ -1722,7 +1724,7 @@
       <c r="P9" s="30"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1">
+    <row r="10" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
@@ -1741,7 +1743,7 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="11" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="29" t="s">
@@ -1770,7 +1772,7 @@
       <c r="P11" s="30"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1">
+    <row r="12" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
@@ -1789,7 +1791,7 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="13" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="29" t="s">
         <v>9</v>
@@ -1817,7 +1819,7 @@
       <c r="P13" s="30"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1">
+    <row r="14" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1835,7 +1837,7 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="15" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="29" t="s">
         <v>30</v>
@@ -1863,7 +1865,7 @@
       <c r="P15" s="30"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1">
+    <row r="16" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1881,7 +1883,7 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="17" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="29" t="s">
         <v>9</v>
@@ -1909,7 +1911,7 @@
       <c r="P17" s="30"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="2:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1">
+    <row r="18" spans="2:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1927,7 +1929,7 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="19" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="29" t="s">
         <v>24</v>
@@ -1955,7 +1957,7 @@
       <c r="P19" s="30"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="2:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1">
+    <row r="20" spans="2:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1973,7 +1975,7 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="21" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="29" t="s">
         <v>15</v>
@@ -1996,13 +1998,13 @@
       <c r="M21" s="30"/>
       <c r="N21" s="4"/>
       <c r="O21" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P21" s="30"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="2:17" ht="15.75" thickBot="1"/>
-    <row r="23" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="22" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="29" t="s">
         <v>37</v>
@@ -2015,22 +2017,22 @@
       <c r="G23" s="8"/>
       <c r="H23" s="3"/>
       <c r="I23" s="31" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="J23" s="32"/>
       <c r="K23" s="4"/>
       <c r="L23" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M23" s="30"/>
       <c r="N23" s="4"/>
       <c r="O23" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P23" s="30"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="2:17" ht="15.75" thickBot="1">
+    <row r="24" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -2047,10 +2049,10 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
     </row>
-    <row r="25" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="25" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="3"/>
@@ -2060,22 +2062,22 @@
       <c r="G25" s="8"/>
       <c r="H25" s="3"/>
       <c r="I25" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J25" s="32"/>
       <c r="K25" s="4"/>
       <c r="L25" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M25" s="30"/>
       <c r="N25" s="4"/>
       <c r="O25" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P25" s="30"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="2:17" ht="15.75" thickBot="1">
+    <row r="26" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -2092,7 +2094,7 @@
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
     </row>
-    <row r="27" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="27" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
@@ -2110,7 +2112,7 @@
       <c r="P27" s="8"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="2:17" ht="15.75" thickBot="1">
+    <row r="28" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -2127,7 +2129,7 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
     </row>
-    <row r="29" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="29" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="7"/>
       <c r="D29" s="8"/>
@@ -2145,7 +2147,7 @@
       <c r="P29" s="8"/>
       <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="2:17" ht="15.75" thickBot="1">
+    <row r="30" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -2162,7 +2164,7 @@
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
     </row>
-    <row r="31" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="31" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
@@ -2180,7 +2182,7 @@
       <c r="P31" s="8"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="2:17" ht="15.75" thickBot="1">
+    <row r="32" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -2197,7 +2199,7 @@
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
     </row>
-    <row r="33" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="33" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="7"/>
       <c r="D33" s="8"/>
@@ -2215,7 +2217,7 @@
       <c r="P33" s="8"/>
       <c r="Q33" s="5"/>
     </row>
-    <row r="34" spans="2:17" ht="15.75" thickBot="1">
+    <row r="34" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -2232,7 +2234,7 @@
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
     </row>
-    <row r="35" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="35" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="7"/>
       <c r="D35" s="8"/>
@@ -2250,7 +2252,7 @@
       <c r="P35" s="8"/>
       <c r="Q35" s="5"/>
     </row>
-    <row r="36" spans="2:17" ht="15.75" thickBot="1">
+    <row r="36" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -2267,7 +2269,7 @@
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
     </row>
-    <row r="37" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="37" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="7"/>
       <c r="D37" s="8"/>
@@ -2285,7 +2287,7 @@
       <c r="P37" s="8"/>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="2:17" ht="15.75" thickBot="1">
+    <row r="38" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -2302,7 +2304,7 @@
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
     </row>
-    <row r="39" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="39" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="7"/>
       <c r="D39" s="8"/>
@@ -2320,7 +2322,7 @@
       <c r="P39" s="8"/>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="2:17" ht="15.75" thickBot="1">
+    <row r="40" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -2337,7 +2339,7 @@
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
     </row>
-    <row r="41" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="41" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="7"/>
       <c r="D41" s="8"/>
@@ -2355,7 +2357,7 @@
       <c r="P41" s="8"/>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="2:17" ht="15.75" thickBot="1">
+    <row r="42" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -2372,7 +2374,7 @@
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
     </row>
-    <row r="43" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="43" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="7"/>
       <c r="D43" s="8"/>
@@ -2390,7 +2392,7 @@
       <c r="P43" s="8"/>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="2:17" ht="15.75" thickBot="1">
+    <row r="44" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -2407,7 +2409,7 @@
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
     </row>
-    <row r="45" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="45" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
       <c r="C45" s="7"/>
       <c r="D45" s="8"/>
@@ -2425,7 +2427,7 @@
       <c r="P45" s="8"/>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="2:17" ht="15.75" thickBot="1">
+    <row r="46" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -2442,7 +2444,7 @@
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
     </row>
-    <row r="47" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="47" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
       <c r="C47" s="7"/>
       <c r="D47" s="8"/>
@@ -2460,7 +2462,7 @@
       <c r="P47" s="8"/>
       <c r="Q47" s="5"/>
     </row>
-    <row r="48" spans="2:17" ht="15.75" thickBot="1">
+    <row r="48" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -2477,7 +2479,7 @@
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
     </row>
-    <row r="49" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="49" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="2"/>
       <c r="C49" s="7"/>
       <c r="D49" s="8"/>
@@ -2495,7 +2497,7 @@
       <c r="P49" s="8"/>
       <c r="Q49" s="5"/>
     </row>
-    <row r="50" spans="2:17" ht="15.75" thickBot="1">
+    <row r="50" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -2512,7 +2514,7 @@
       <c r="P50" s="3"/>
       <c r="Q50" s="3"/>
     </row>
-    <row r="51" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="51" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="2"/>
       <c r="C51" s="7"/>
       <c r="D51" s="8"/>
@@ -2530,7 +2532,7 @@
       <c r="P51" s="8"/>
       <c r="Q51" s="5"/>
     </row>
-    <row r="52" spans="2:17" ht="15.75" thickBot="1">
+    <row r="52" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -2547,7 +2549,7 @@
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
     </row>
-    <row r="53" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1">
+    <row r="53" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="2"/>
       <c r="C53" s="7"/>
       <c r="D53" s="8"/>
@@ -2632,12 +2634,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Finalizado fluxograma Atualizado linhas dos graficos estratificados por área, arquivo de dispensa
</commit_message>
<xml_diff>
--- a/SICOP 1.xlsx
+++ b/SICOP 1.xlsx
@@ -546,6 +546,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -560,30 +584,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1512,7 +1512,7 @@
   <dimension ref="A2:Q53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I25" sqref="I25:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,59 +1573,59 @@
     <row r="4" spans="1:17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="26"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="15"/>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="28"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="16"/>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="26"/>
+      <c r="M4" s="25"/>
       <c r="N4" s="16"/>
-      <c r="O4" s="25" t="s">
+      <c r="O4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="26"/>
+      <c r="P4" s="25"/>
       <c r="Q4" s="17"/>
     </row>
     <row r="5" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="21"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="21"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="15"/>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="23"/>
+      <c r="J5" s="31"/>
       <c r="K5" s="18"/>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="21"/>
+      <c r="M5" s="29"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="24" t="s">
+      <c r="O5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="21"/>
+      <c r="P5" s="29"/>
       <c r="Q5" s="19"/>
     </row>
     <row r="6" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1650,30 +1650,30 @@
     <row r="7" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="21"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="30"/>
+      <c r="G7" s="21"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="32"/>
+      <c r="J7" s="23"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="29" t="s">
+      <c r="L7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="30"/>
+      <c r="M7" s="21"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="29" t="s">
+      <c r="O7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="30"/>
+      <c r="P7" s="21"/>
       <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1698,30 +1698,30 @@
     <row r="9" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="30"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="30"/>
+      <c r="G9" s="21"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="31" t="s">
+      <c r="I9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="32"/>
+      <c r="J9" s="23"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="29" t="s">
+      <c r="L9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="30"/>
+      <c r="M9" s="21"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="29" t="s">
+      <c r="O9" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P9" s="30"/>
+      <c r="P9" s="21"/>
       <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1746,30 +1746,30 @@
     <row r="11" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="21"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="32"/>
+      <c r="J11" s="23"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="29" t="s">
+      <c r="L11" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="M11" s="30"/>
+      <c r="M11" s="21"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="29" t="s">
+      <c r="O11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="P11" s="30"/>
+      <c r="P11" s="21"/>
       <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1793,30 +1793,30 @@
     </row>
     <row r="13" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="30"/>
+      <c r="D13" s="21"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="30"/>
+      <c r="G13" s="21"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="31" t="s">
+      <c r="I13" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="32"/>
+      <c r="J13" s="23"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="29" t="s">
+      <c r="L13" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="M13" s="30"/>
+      <c r="M13" s="21"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="29" t="s">
+      <c r="O13" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="P13" s="30"/>
+      <c r="P13" s="21"/>
       <c r="Q13" s="5"/>
     </row>
     <row r="14" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1839,30 +1839,30 @@
     </row>
     <row r="15" spans="1:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="30"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="30"/>
+      <c r="G15" s="21"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="32"/>
+      <c r="J15" s="23"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="29" t="s">
+      <c r="L15" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="30"/>
+      <c r="M15" s="21"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="29" t="s">
+      <c r="O15" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="P15" s="30"/>
+      <c r="P15" s="21"/>
       <c r="Q15" s="5"/>
     </row>
     <row r="16" spans="1:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1885,30 +1885,30 @@
     </row>
     <row r="17" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="30"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="21"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="31" t="s">
+      <c r="I17" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="32"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="29" t="s">
+      <c r="L17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="30"/>
+      <c r="M17" s="21"/>
       <c r="N17" s="4"/>
-      <c r="O17" s="29" t="s">
+      <c r="O17" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P17" s="30"/>
+      <c r="P17" s="21"/>
       <c r="Q17" s="5"/>
     </row>
     <row r="18" spans="2:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1931,30 +1931,30 @@
     </row>
     <row r="19" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="30"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="30"/>
+      <c r="G19" s="21"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="31" t="s">
+      <c r="I19" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="J19" s="32"/>
+      <c r="J19" s="23"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="29" t="s">
+      <c r="L19" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="M19" s="30"/>
+      <c r="M19" s="21"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="29" t="s">
+      <c r="O19" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="P19" s="30"/>
+      <c r="P19" s="21"/>
       <c r="Q19" s="5"/>
     </row>
     <row r="20" spans="2:17" s="6" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1977,59 +1977,59 @@
     </row>
     <row r="21" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="30"/>
+      <c r="D21" s="21"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="29" t="s">
+      <c r="F21" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="30"/>
+      <c r="G21" s="21"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="J21" s="32"/>
+      <c r="J21" s="23"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="29" t="s">
+      <c r="L21" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="30"/>
+      <c r="M21" s="21"/>
       <c r="N21" s="4"/>
-      <c r="O21" s="29" t="s">
+      <c r="O21" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="P21" s="30"/>
+      <c r="P21" s="21"/>
       <c r="Q21" s="5"/>
     </row>
     <row r="22" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="30"/>
+      <c r="D23" s="21"/>
       <c r="E23" s="3"/>
       <c r="F23" s="7" t="s">
         <v>33</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="31" t="s">
+      <c r="I23" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="J23" s="32"/>
+      <c r="J23" s="23"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="29" t="s">
+      <c r="L23" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="M23" s="30"/>
+      <c r="M23" s="21"/>
       <c r="N23" s="4"/>
-      <c r="O23" s="29" t="s">
+      <c r="O23" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="P23" s="30"/>
+      <c r="P23" s="21"/>
       <c r="Q23" s="5"/>
     </row>
     <row r="24" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2051,30 +2051,30 @@
     </row>
     <row r="25" spans="2:17" s="6" customFormat="1" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="30"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="3"/>
       <c r="F25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="31" t="s">
+      <c r="I25" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="J25" s="32"/>
+      <c r="J25" s="23"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="29" t="s">
+      <c r="L25" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="M25" s="30"/>
+      <c r="M25" s="21"/>
       <c r="N25" s="4"/>
-      <c r="O25" s="29" t="s">
+      <c r="O25" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="P25" s="30"/>
+      <c r="P25" s="21"/>
       <c r="Q25" s="5"/>
     </row>
     <row r="26" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2569,6 +2569,56 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="O19:P19"/>
     <mergeCell ref="L23:M23"/>
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="O23:P23"/>
@@ -2577,56 +2627,6 @@
     <mergeCell ref="L25:M25"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="O5:P5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>